<commit_message>
things that haven't been committed, but already used for thesis
</commit_message>
<xml_diff>
--- a/Datasets/2nd Analysis Datasets/Results/SentiStrength/Bias_Dataset_SentiStrength.xlsx
+++ b/Datasets/2nd Analysis Datasets/Results/SentiStrength/Bias_Dataset_SentiStrength.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\2nd Analysis Datasets\Results\SentiStrength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE21923-029B-4E09-94FE-020235E325FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C8998-266B-4E61-907F-A2DAA9F6BFA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{836568EA-315C-4664-B2E1-8F0BCE856F54}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>Positive</t>
   </si>
@@ -270,6 +270,18 @@
   </si>
   <si>
     <t>Polarity</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>FN</t>
   </si>
 </sst>
 </file>
@@ -625,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C97543-BE71-4AD8-B417-A4BF8EB6C48F}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +652,7 @@
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -659,8 +671,32 @@
       <c r="F1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -680,8 +716,40 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="b">
+        <f>IF(AND(A2=-1,F2=-1),"TP")</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <f>IF(AND(A2=1,F2=-1),"FP")</f>
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <f>IF(AND(A2=1,F2=1),"TN")</f>
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <f>IF(AND(A2=-1,F2=1),"FN")</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>COUNTIF(H2:H200,"TP")</f>
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <f>COUNTIF(I2:I200,"FP")</f>
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <f>COUNTIF(J2:J200,"TN")</f>
+        <v>24</v>
+      </c>
+      <c r="P2">
+        <f>COUNTIF(K2:K200,"FN")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -701,8 +769,24 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="b">
+        <f t="shared" ref="H3:H66" si="1">IF(AND(A3=-1,F3=-1),"TP")</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <f t="shared" ref="I3:I66" si="2">IF(AND(A3=1,F3=-1),"FP")</f>
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <f t="shared" ref="J3:J66" si="3">IF(AND(A3=1,F3=1),"TN")</f>
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <f t="shared" ref="K3:K66" si="4">IF(AND(A3=-1,F3=1),"FN")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -722,8 +806,24 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -743,8 +843,24 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-1</v>
       </c>
@@ -764,8 +880,24 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-1</v>
       </c>
@@ -785,8 +917,24 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>FN</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-1</v>
       </c>
@@ -806,8 +954,24 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -827,8 +991,24 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K9" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -848,8 +1028,24 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -869,8 +1065,24 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -890,8 +1102,24 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -911,8 +1139,24 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -932,8 +1176,24 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-1</v>
       </c>
@@ -953,8 +1213,24 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-1</v>
       </c>
@@ -974,8 +1250,24 @@
       <c r="F16">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>TP</v>
+      </c>
+      <c r="I16" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -995,8 +1287,24 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1016,8 +1324,24 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1037,8 +1361,24 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1058,8 +1398,24 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-1</v>
       </c>
@@ -1079,8 +1435,24 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>FN</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1100,8 +1472,24 @@
       <c r="F22">
         <v>-1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v>FP</v>
+      </c>
+      <c r="J22" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-1</v>
       </c>
@@ -1121,8 +1509,24 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1142,8 +1546,24 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1</v>
       </c>
@@ -1163,8 +1583,24 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1184,8 +1620,24 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1205,8 +1657,24 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1226,8 +1694,24 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K28" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-1</v>
       </c>
@@ -1247,8 +1731,24 @@
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>FN</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1268,8 +1768,24 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K30" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-1</v>
       </c>
@@ -1289,8 +1805,24 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-1</v>
       </c>
@@ -1310,8 +1842,24 @@
       <c r="F32">
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>TP</v>
+      </c>
+      <c r="I32" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1331,8 +1879,24 @@
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K33" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1352,8 +1916,24 @@
       <c r="F34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K34" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1373,8 +1953,24 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H35" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K35" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1394,8 +1990,24 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K36" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1415,8 +2027,24 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H37" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1436,8 +2064,24 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K38" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-1</v>
       </c>
@@ -1457,8 +2101,24 @@
       <c r="F39">
         <v>-1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v>TP</v>
+      </c>
+      <c r="I39" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-1</v>
       </c>
@@ -1478,8 +2138,24 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1499,8 +2175,24 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H41" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K41" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1520,8 +2212,24 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K42" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1541,8 +2249,24 @@
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H43" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K43" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1562,8 +2286,24 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K44" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-1</v>
       </c>
@@ -1583,8 +2323,24 @@
       <c r="F45">
         <v>-1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v>TP</v>
+      </c>
+      <c r="I45" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J45" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K45" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1604,8 +2360,24 @@
       <c r="F46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K46" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1625,8 +2397,24 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K47" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-1</v>
       </c>
@@ -1646,8 +2434,24 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I48" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J48" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K48" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1667,8 +2471,24 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J49" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1688,8 +2508,24 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H50" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J50" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -1709,8 +2545,24 @@
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H51" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K51" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1730,8 +2582,24 @@
       <c r="F52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H52" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K52" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1751,8 +2619,24 @@
       <c r="F53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H53" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K53" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1772,8 +2656,24 @@
       <c r="F54">
         <v>-1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H54" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="2"/>
+        <v>FP</v>
+      </c>
+      <c r="J54" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K54" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-1</v>
       </c>
@@ -1793,8 +2693,24 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H55" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I55" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J55" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K55" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1814,8 +2730,24 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H56" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J56" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K56" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-1</v>
       </c>
@@ -1835,8 +2767,24 @@
       <c r="F57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H57" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J57" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="4"/>
+        <v>FN</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-1</v>
       </c>
@@ -1856,8 +2804,24 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H58" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I58" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J58" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K58" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1877,8 +2841,24 @@
       <c r="F59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H59" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K59" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-1</v>
       </c>
@@ -1898,8 +2878,24 @@
       <c r="F60">
         <v>-1</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H60" t="str">
+        <f t="shared" si="1"/>
+        <v>TP</v>
+      </c>
+      <c r="I60" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J60" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K60" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-1</v>
       </c>
@@ -1919,8 +2915,24 @@
       <c r="F61">
         <v>-1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H61" t="str">
+        <f t="shared" si="1"/>
+        <v>TP</v>
+      </c>
+      <c r="I61" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J61" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K61" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -1940,8 +2952,24 @@
       <c r="F62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H62" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I62" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J62" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K62" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1961,8 +2989,24 @@
       <c r="F63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H63" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K63" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1</v>
       </c>
@@ -1982,8 +3026,24 @@
       <c r="F64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H64" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K64" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1</v>
       </c>
@@ -2003,8 +3063,24 @@
       <c r="F65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H65" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I65" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K65" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1</v>
       </c>
@@ -2024,8 +3100,24 @@
       <c r="F66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H66" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="3"/>
+        <v>TN</v>
+      </c>
+      <c r="K66" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-1</v>
       </c>
@@ -2039,14 +3131,30 @@
         <v>-1</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E68" si="1">C67+D67</f>
+        <f t="shared" ref="E67:E68" si="5">C67+D67</f>
         <v>2</v>
       </c>
       <c r="F67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H67" t="b">
+        <f t="shared" ref="H67:H68" si="6">IF(AND(A67=-1,F67=-1),"TP")</f>
+        <v>0</v>
+      </c>
+      <c r="I67" t="b">
+        <f t="shared" ref="I67:I68" si="7">IF(AND(A67=1,F67=-1),"FP")</f>
+        <v>0</v>
+      </c>
+      <c r="J67" t="b">
+        <f t="shared" ref="J67:J68" si="8">IF(AND(A67=1,F67=1),"TN")</f>
+        <v>0</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K68" si="9">IF(AND(A67=-1,F67=1),"FN")</f>
+        <v>FN</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -2060,10 +3168,26 @@
         <v>-1</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="H68" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I68" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J68" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K68" t="b">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>